<commit_message>
added comments and requirements.txt file
</commit_message>
<xml_diff>
--- a/City_temperatures.xlsx
+++ b/City_temperatures.xlsx
@@ -1,88 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23107"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3BB4FAF-F83D-4DB4-9621-B36EF9F8BB69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="1" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191028" fullCalcOnLoad="1" calcCompleted="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>City Name</t>
-  </si>
-  <si>
-    <t>Temperature in F</t>
-  </si>
-  <si>
-    <t>Temperature in C</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>New Delhi</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>Possible Cities</t>
-  </si>
-  <si>
-    <t>The API can provide data of almost every city acroos the globe.</t>
-  </si>
-  <si>
-    <t>The program can be terminated by pressing CTRL + C</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -101,22 +56,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -416,71 +430,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="15.28515625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>289.87</v>
-      </c>
-      <c r="C3">
-        <v>143.26111111111109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>City Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Temperature in F</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Temperature in C</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>290.52</v>
+      </c>
+      <c r="C3" t="n">
+        <v>143.6222222222222</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>New Delhi</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>308.58</v>
       </c>
-      <c r="C4">
-        <v>153.65555555555559</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
+      <c r="C4" t="n">
+        <v>153.6555555555556</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>295.82</v>
       </c>
-      <c r="C5">
-        <v>146.56666666666669</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>301.04000000000002</v>
-      </c>
-      <c r="C6">
+      <c r="C5" t="n">
+        <v>146.5666666666667</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Singapore</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>301.04</v>
+      </c>
+      <c r="C6" t="n">
         <v>149.4666666666667</v>
       </c>
     </row>
@@ -490,24 +522,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" customWidth="1"/>
+    <col width="55.5703125" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Possible Cities</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>The API can provide data of almost every city acroos the globe.</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -516,16 +558,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>The program can be terminated by pressing CTRL + C</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>